<commit_message>
fixed promt and normalizing
</commit_message>
<xml_diff>
--- a/Output/CVs_Info_Extracted.xlsx
+++ b/Output/CVs_Info_Extracted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,120 +441,75 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Education Bachelor University</t>
+          <t>University Education</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Education Bachelor GPA</t>
+          <t>Years of Experience</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Education Bachelor Major</t>
+          <t>Experience Companies</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Education Bachelor Graduation Date</t>
+          <t>Top 5 Responsibilities/Projects</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Education Masters University</t>
+          <t>Top 5 Courses/Certifications</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Education Masters GPA</t>
+          <t>Top 3 Technical Skills</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Education Masters Major</t>
+          <t>Top 3 Soft Skills</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Education Masters Graduation Date</t>
+          <t>Current Employment Status</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Education PhD University</t>
+          <t>Nationality</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Education PhD GPA</t>
+          <t>Current Residence</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Education PhD Major</t>
+          <t>Suitable Position</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Education PhD Graduation Date</t>
+          <t>Languages</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Years of Experience</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Experience Companies</t>
+          <t>Phone Number</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Top 5 Responsibilities/Projects</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Top 5 Courses/Certifications</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Top 3 Technical Skills</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Top 3 Soft Skills</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Current Employment Status</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Nationality</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Current Residence</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Suitable Position</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Candidate Rating (Out of 10)</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>All_Info_JSON</t>
         </is>
@@ -566,91 +521,76 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ali Abuharb's CV.pdf</t>
+          <t>Michael-Conner.pdf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>King Fahd University of Petroleum &amp; Minerals</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3.03/4</t>
-        </is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Management Information Systems</t>
+          <t>['GEV Wind Power-Siemens Blade Factory', 'Geofrac Ltd-Gateshead', 'Plumbing and heating supplies-Gateshead', 'Aldi', 'Carillion']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>May, 2020</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+          <t>['Inspecting, maintaining, and repairing Siemens wind turbine blades', 'Delivering parcels for Amazon through Geofrac Ltd in a 3.5T van', 'Managing warehouse operations including goods in, goods out, and stock levels', 'Being responsible for the store as a Deputy Manager at Aldi', 'Completing theory and practical tests to gain NVQ level 2 in bricklaying']</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>['GWO Sea Survival', 'GWO Blade Repair', 'GWO Manual Handling', 'GWO First Aid', 'GWO Advanced Rescue Training']</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>['Effective communication', 'Organizational skills', 'Customer service']</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="n">
-        <v>3</v>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Blaydon, ENG NE21 NE21</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>[{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 0.7}, {'position': 'Blade Repair', 'suitability': 0.9}]</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>michaelconner321@gmail.com</t>
+        </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>['Lean', 'Ministry of Interior']</t>
+          <t>+44 7932 638510</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>['Led Resources on Data Projects', 'NLP Projects', 'Images Data Projects', 'DRG Engine Development', 'Data Detection Engine Development']</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>['Deep Learning 5 months Specialization', 'Spark and Python for Big Data with PySpark', 'Introduction to Apache NiFi|Cloudera DataFlow | HDF 2.0', 'Scientific Computing with Python', 'Nanodegree, Machine Learning']</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>['Deep Learning', 'Machine Learning', 'NLP']</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>['Leadership', 'Project Management', 'Time Management']</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Saudi Arabian</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Riyadh</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>Data Scientist</t>
-        </is>
-      </c>
-      <c r="Y2" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>{'Education Bachelor University': 'King Fahd University of Petroleum &amp; Minerals', 'Education Bachelor GPA': '3.03/4', 'Education Bachelor Major': 'Management Information Systems', 'Education Bachelor Graduation Date': 'May, 2020', 'Education Masters University': '', 'Education Masters GPA': '', 'Education Masters Major': '', 'Education Masters Graduation Date': '', 'Education PhD University': '', 'Education PhD GPA': '', 'Education PhD Major': '', 'Education PhD Graduation Date': '', 'Years of Experience': '3', 'Experience Companies': ['Lean', 'Ministry of Interior'], 'Top 5 Responsibilities/Projects': ['Led Resources on Data Projects', 'NLP Projects', 'Images Data Projects', 'DRG Engine Development', 'Data Detection Engine Development'], 'Top 5 Courses/Certifications': ['Deep Learning 5 months Specialization', 'Spark and Python for Big Data with PySpark', 'Introduction to Apache NiFi|Cloudera DataFlow | HDF 2.0', 'Scientific Computing with Python', 'Nanodegree, Machine Learning'], 'Top 3 Technical Skills': ['Deep Learning', 'Machine Learning', 'NLP'], 'Top 3 Soft Skills': ['Leadership', 'Project Management', 'Time Management'], 'Current Employment Status': 'Full-time', 'Nationality': 'Saudi Arabian', 'Current Residence': 'Riyadh', 'Suitable Position': 'Data Scientist', 'Candidate Rating (Out of 10)': '8'}</t>
+          <t>{'University Education': [], 'Years of Experience': 8, 'Experience Companies': ['GEV Wind Power-Siemens Blade Factory', 'Geofrac Ltd-Gateshead', 'Plumbing and heating supplies-Gateshead', 'Aldi', 'Carillion'], 'Top 5 Responsibilities/Projects': ['Inspecting, maintaining, and repairing Siemens wind turbine blades', 'Delivering parcels for Amazon through Geofrac Ltd in a 3.5T van', 'Managing warehouse operations including goods in, goods out, and stock levels', 'Being responsible for the store as a Deputy Manager at Aldi', 'Completing theory and practical tests to gain NVQ level 2 in bricklaying'], 'Top 5 Courses/Certifications': ['GWO Sea Survival', 'GWO Blade Repair', 'GWO Manual Handling', 'GWO First Aid', 'GWO Advanced Rescue Training'], 'Top 3 Technical Skills': [], 'Top 3 Soft Skills': ['Effective communication', 'Organizational skills', 'Customer service'], 'Current Employment Status': 'Full-time', 'Nationality': '', 'Current Residence': 'Blaydon, ENG NE21 NE21', 'Suitable Position': [{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 0.7}, {'position': 'Blade Repair', 'suitability': 0.9}], 'Languages': [], 'Email': 'michaelconner321@gmail.com', 'Phone Number': '+44 7932 638510'}</t>
         </is>
       </c>
     </row>
@@ -660,99 +600,76 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dmitry Odinoky CV.pdf</t>
+          <t>Miguel Monteiro CV  2025.pdf</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Rigas Tehniska universitate (Riga Technical University)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>[{'university': 'Gondomar secondary school', 'year': '2007', 'type': 'A Level - Course Science and Technology'}, {'university': 'CINDOR, Centre For the Industry of Jewellery and Watchmaking', 'year': '2007', 'type': 'level 3 Jeweller course, with a CAD and Metal Technology component'}]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>14</v>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Robotics and Artificial Intelligence</t>
+          <t>['Fortil- Offshore-France PGB', 'Tubestar-Offshore-Italy', 'ASP International-offshore Netherlands', 'Metiba', 'PATORRA']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>June, 2020</t>
+          <t>['Certification works on WTG service Lift, anchor points, fire extinguishers and Chain hoist', 'Lifting Gear equipment’s inspection with NDT for shelf Drilling', 'Laying cables between platforms in an HKZ- windfarm offshore park in rotation 2/2', 'Led a team in different works such as rescue work, inspection of structures with NDT techniques, preventive maintenance with welding and cutting', 'Led a team on site, in the construction and assembly of artificial stranded structures in metal, wood and composite materials, rope Access']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Rigas Tehniska universitate (Riga Technical University)</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>['IRATA L3/ 135816', 'END-1597 VISUAL TESTING L2', 'END-2037 Magnetic particle Testing L2', 'VCA SUPERVISOR 946863 .30066540', 'Atex atmospheres']</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['Rope Access IRATA L3', 'VT MPI L2 Inspector', 'Welder']</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Robotics and Artificial Intelligence</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>June, 2023</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>13</v>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Portuguese</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Oporto</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>[{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 0.9}, {'position': 'Blade Repair', 'suitability': 0.7}]</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>['Portuguese', 'English', 'Spanish']</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Mikemota9@gmail.com</t>
+        </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>['Sonarworks', 'Yamaha Music Europe', 'Dynamic Records', 'SIA Dinamic Records', 'Radio PIK']</t>
+          <t>+00351919814617</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>['Internal prototyping, development, and testing of SoundID Reference', 'Development and testing of VoiceAI and SoundID™ Audio Personalization App', 'Supporting product dealers through email requests', 'Becoming the only Ableton &amp; Steinberg certified tutor in Baltics', 'Leading music production school and recording studio in Riga']</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>['Ableton Certified Trainer', 'Audio Signal Processing for Music Applications (Universitat Pompeu Fabra of Barcelona)']</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>['Data Science', 'Machine Learning', 'Python']</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>['Project Management', 'Education', 'Sound Design']</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>Latvian</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>Riga, LV</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>Data Scientist</t>
-        </is>
-      </c>
-      <c r="Y3" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>{'Education Bachelor University': 'Rigas Tehniska universitate (Riga Technical University)', 'Education Bachelor GPA': '', 'Education Bachelor Major': 'Robotics and Artificial Intelligence', 'Education Bachelor Graduation Date': 'June, 2020', 'Education Masters University': 'Rigas Tehniska universitate (Riga Technical University)', 'Education Masters GPA': '', 'Education Masters Major': 'Robotics and Artificial Intelligence', 'Education Masters Graduation Date': 'June, 2023', 'Education PhD University': '', 'Education PhD GPA': '', 'Education PhD Major': '', 'Education PhD Graduation Date': '', 'Years of Experience': '13', 'Experience Companies': ['Sonarworks', 'Yamaha Music Europe', 'Dynamic Records', 'SIA Dinamic Records', 'Radio PIK'], 'Top 5 Responsibilities/Projects': ['Internal prototyping, development, and testing of SoundID Reference', 'Development and testing of VoiceAI and SoundID™ Audio Personalization App', 'Supporting product dealers through email requests', 'Becoming the only Ableton &amp; Steinberg certified tutor in Baltics', 'Leading music production school and recording studio in Riga'], 'Top 5 Courses/Certifications': ['Ableton Certified Trainer', 'Audio Signal Processing for Music Applications (Universitat Pompeu Fabra of Barcelona)'], 'Top 3 Technical Skills': ['Data Science', 'Machine Learning', 'Python'], 'Top 3 Soft Skills': ['Project Management', 'Education', 'Sound Design'], 'Current Employment Status': 'Full-time', 'Nationality': 'Latvian', 'Current Residence': 'Riga, LV', 'Suitable Position': 'Data Scientist', 'Candidate Rating (Out of 10)': '8'}</t>
+          <t>{'University Education': [{'university': 'Gondomar secondary school', 'year': '2007', 'type': 'A Level - Course Science and Technology'}, {'university': 'CINDOR, Centre For the Industry of Jewellery and Watchmaking', 'year': '2007', 'type': 'level 3 Jeweller course, with a CAD and Metal Technology component'}], 'Years of Experience': '14', 'Experience Companies': ['Fortil- Offshore-France PGB', 'Tubestar-Offshore-Italy', 'ASP International-offshore Netherlands', 'Metiba', 'PATORRA'], 'Top 5 Responsibilities/Projects': ['Certification works on WTG service Lift, anchor points, fire extinguishers and Chain hoist', 'Lifting Gear equipment’s inspection with NDT for shelf Drilling', 'Laying cables between platforms in an HKZ- windfarm offshore park in rotation 2/2', 'Led a team in different works such as rescue work, inspection of structures with NDT techniques, preventive maintenance with welding and cutting', 'Led a team on site, in the construction and assembly of artificial stranded structures in metal, wood and composite materials, rope Access'], 'Top 5 Courses/Certifications': ['IRATA L3/ 135816', 'END-1597 VISUAL TESTING L2', 'END-2037 Magnetic particle Testing L2', 'VCA SUPERVISOR 946863 .30066540', 'Atex atmospheres'], 'Top 3 Technical Skills': ['Rope Access IRATA L3', 'VT MPI L2 Inspector', 'Welder'], 'Top 3 Soft Skills': [], 'Current Employment Status': '', 'Nationality': 'Portuguese', 'Current Residence': 'Oporto', 'Suitable Position': [{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 0.9}, {'position': 'Blade Repair', 'suitability': 0.7}], 'Languages': ['Portuguese', 'English', 'Spanish'], 'Email': 'Mikemota9@gmail.com', 'Phone Number': '+00351919814617'}</t>
         </is>
       </c>
     </row>
@@ -762,85 +679,242 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Deemah_Alabdulaali_Resume.pdf</t>
+          <t>milan-k-o.pdf</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>King Saud University - Riyadh</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4.99/5.00</t>
-        </is>
+          <t>[{'university': 'St,Francis Assisi Higher Secondary School,Arthunkal', 'year': '', 'type': 'Bachelor'}, {'university': 'St,Francis Assisi Higher Secondary School,Arthunkal', 'year': '', 'type': 'Bachelor'}]</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Information Systems</t>
+          <t>['Aries Marine', 'TATA STEEL']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>December, 2018</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+          <t>['UT Inspection', 'Structure Welding', 'Gas Cutting', 'Sheet Replacement', 'Clamp Fixing']</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>['Caring about others', 'Comforting people when they need it', 'Conflict management and resolution skill']</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="n">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Indian</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Kurisunkal,Arthunkal P O Cherthala,Alappuzha</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>[{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 1.0}, {'position': 'Blade Repair', 'suitability': 0.7}]</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>milankurisunkal1212@gmail.com</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>7025973882</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>{'University Education': [{'university': 'St,Francis Assisi Higher Secondary School,Arthunkal', 'year': '', 'type': 'Bachelor'}, {'university': 'St,Francis Assisi Higher Secondary School,Arthunkal', 'year': '', 'type': 'Bachelor'}], 'Years of Experience': '0', 'Experience Companies': ['Aries Marine', 'TATA STEEL'], 'Top 5 Responsibilities/Projects': ['UT Inspection', 'Structure Welding', 'Gas Cutting', 'Sheet Replacement', 'Clamp Fixing'], 'Top 5 Courses/Certifications': [], 'Top 3 Technical Skills': [], 'Top 3 Soft Skills': ['Caring about others', 'Comforting people when they need it', 'Conflict management and resolution skill'], 'Current Employment Status': '', 'Nationality': 'Indian', 'Current Residence': 'Kurisunkal,Arthunkal P O Cherthala,Alappuzha', 'Suitable Position': [{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 1.0}, {'position': 'Blade Repair', 'suitability': 0.7}], 'Languages': [], 'Email': 'milankurisunkal1212@gmail.com', 'Phone Number': '7025973882'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mohamed shalaby cv.pdf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[{'university': 'Al Azhar University', 'year': '2007', 'type': 'Bachelor'}]</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>15</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['YKR (ARISE GLOBAL branch in KAZAKHSTAN)', 'Inspecta International Company', 'IMW', 'QUALITY CONTROL - CAIRO, EGYPT', 'Petrojet Company']</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['Supervision for rope access team making Radiographic testing at KTL plant', 'Supervisor of irata rope access team doing NDT activities using rope access for Inspection', 'Follow up all the NDT activities using rope access for Inspection', 'Follow up all the NDT activities using rope access for Inspection', 'Making maintenances for all GUPCO platforms']</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['Certified Welding Inspector (CWI)', 'IRATA Rope access level 3', 'Basic H2S traninig OPITO course', 'BOSIET (with EBS)', 'Level (Il) Ultrasonic Testing ASNT (UT)']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['NDT', 'Rope Access', 'Radiographic Testing']</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>['Leadership', 'Communication', 'Problem Solving']</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Egyptian</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Basyon - El Gharbia - EGYPT</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>['Arabic', 'English']</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Manegerway@gmail.com</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>+201061799019</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>{'University Education': [{'university': 'Al Azhar University', 'year': '2007', 'type': 'Bachelor'}], 'Years of Experience': '15', 'Experience Companies': ['YKR (ARISE GLOBAL branch in KAZAKHSTAN)', 'Inspecta International Company', 'IMW', 'QUALITY CONTROL - CAIRO, EGYPT', 'Petrojet Company'], 'Top 5 Responsibilities/Projects': ['Supervision for rope access team making Radiographic testing at KTL plant', 'Supervisor of irata rope access team doing NDT activities using rope access for Inspection', 'Follow up all the NDT activities using rope access for Inspection', 'Follow up all the NDT activities using rope access for Inspection', 'Making maintenances for all GUPCO platforms'], 'Top 5 Courses/Certifications': ['Certified Welding Inspector (CWI)', 'IRATA Rope access level 3', 'Basic H2S traninig OPITO course', 'BOSIET (with EBS)', 'Level (Il) Ultrasonic Testing ASNT (UT)'], 'Top 3 Technical Skills': ['NDT', 'Rope Access', 'Radiographic Testing'], 'Top 3 Soft Skills': ['Leadership', 'Communication', 'Problem Solving'], 'Current Employment Status': 'Full-time', 'Nationality': 'Egyptian', 'Current Residence': 'Basyon - El Gharbia - EGYPT', 'Suitable Position': [], 'Languages': ['Arabic', 'English'], 'Email': 'Manegerway@gmail.com', 'Phone Number': '+201061799019'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>['Lean Business Services, Riyadh', 'Confidential, Rivadh']</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>['Managing a team of 6 data scientists and machine learning engineers', 'Leading and planning +5 data and machine learning projects from an initial idea to deployment', 'Collaborating with business to identify and prioritize business problems that can be solved with machine learning', 'Identifying and evaluating new machine learning technologies', 'Hands on development of machine learning projects']</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Michael fife CV.pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>['Tensorflow/keras', 'PyTorch', 'NLTK']</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>['Communication', 'Leadership', 'Problem solving']</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
+      <c r="D6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['GEV Onshore/Offshore', 'Self UK/EU', 'Texo', 'SMC (Specialist Marine UK/EU Consultant)', 'Nissan UK', 'The School Outfit', 'Signal Plastics UK']</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['Conducted detailed inspections of wind turbine blades for leading edge erosion using rope access techniques', 'Fibre glass repairs using composite patches', 'Performed remediation and repair of eroded blade edge, including surface preparation, filling and application of protective coating', 'Application of LEPO9', "Installation of VG's"]</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['lrata Level 3 Cert', 'Siemens Spot on metal', 'Siemens E learing', 'Epoxy Safety', 'CCNSG Safety Passport']</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['Rope Access Techniques', 'Wind Turbine Maintenance', 'Painting Projects']</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>['Ability to Work in a Team', 'Communication Skills', 'Adaptability']</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Full-time</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>Riyadh, Saudi Arabia</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Data Scientist</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>{'Education Bachelor University': 'King Saud University - Riyadh', 'Education Bachelor GPA': '4.99/5.00', 'Education Bachelor Major': 'Information Systems', 'Education Bachelor Graduation Date': 'December, 2018', 'Education Masters University': '', 'Education Masters GPA': '', 'Education Masters Major': '', 'Education Masters Graduation Date': '', 'Education PhD University': '', 'Education PhD GPA': '', 'Education PhD Major': '', 'Education PhD Graduation Date': '', 'Years of Experience': '4', 'Experience Companies': ['Lean Business Services, Riyadh', 'Confidential, Rivadh'], 'Top 5 Responsibilities/Projects': ['Managing a team of 6 data scientists and machine learning engineers', 'Leading and planning +5 data and machine learning projects from an initial idea to deployment', 'Collaborating with business to identify and prioritize business problems that can be solved with machine learning', 'Identifying and evaluating new machine learning technologies', 'Hands on development of machine learning projects'], 'Top 5 Courses/Certifications': [], 'Top 3 Technical Skills': ['Tensorflow/keras', 'PyTorch', 'NLTK'], 'Top 3 Soft Skills': ['Communication', 'Leadership', 'Problem solving'], 'Current Employment Status': 'Full-time', 'Nationality': '', 'Current Residence': 'Riyadh, Saudi Arabia', 'Suitable Position': 'Data Scientist', 'Candidate Rating (Out of 10)': ''}</t>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Sunderland, United Kingdom</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>[{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 0.9}, {'position': 'Blade Repair', 'suitability': 0.7}]</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>michaelfife87@gmail.com</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>07826615265</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>{'University Education': [], 'Years of Experience': 16, 'Experience Companies': ['GEV Onshore/Offshore', 'Self UK/EU', 'Texo', 'SMC (Specialist Marine UK/EU Consultant)', 'Nissan UK', 'The School Outfit', 'Signal Plastics UK'], 'Top 5 Responsibilities/Projects': ['Conducted detailed inspections of wind turbine blades for leading edge erosion using rope access techniques', 'Fibre glass repairs using composite patches', 'Performed remediation and repair of eroded blade edge, including surface preparation, filling and application of protective coating', 'Application of LEPO9', "Installation of VG's"], 'Top 5 Courses/Certifications': ['lrata Level 3 Cert', 'Siemens Spot on metal', 'Siemens E learing', 'Epoxy Safety', 'CCNSG Safety Passport'], 'Top 3 Technical Skills': ['Rope Access Techniques', 'Wind Turbine Maintenance', 'Painting Projects'], 'Top 3 Soft Skills': ['Ability to Work in a Team', 'Communication Skills', 'Adaptability'], 'Current Employment Status': 'Full-time', 'Nationality': 'United Kingdom', 'Current Residence': 'Sunderland, United Kingdom', 'Suitable Position': [{'position': 'MARITIME', 'suitability': 0.8}, {'position': 'IRATA', 'suitability': 0.9}, {'position': 'Blade Repair', 'suitability': 0.7}], 'Languages': [], 'Email': 'michaelfife87@gmail.com', 'Phone Number': '07826615265'}</t>
         </is>
       </c>
     </row>

</xml_diff>